<commit_message>
add ca 4700 files
add ca 4700 files
</commit_message>
<xml_diff>
--- a/Example2.xlsx
+++ b/Example2.xlsx
@@ -25,34 +25,34 @@
     <t>set()</t>
   </si>
   <si>
-    <t>{'journey)', '(the'}</t>
-  </si>
-  <si>
-    <t>{'dinnertimethe', 'lightsthe', 'spritz', 'aperol', 'usthe', 'hotelwe', 'himthey', 'spritzi', 'lemoncello'}</t>
-  </si>
-  <si>
-    <t>{'standardtoiletries', 'aminta', 'noneall', 'viewbut', 'excellentimmaculately', 'alsothe'}</t>
-  </si>
-  <si>
-    <t>{'areathe', 'â‚¬20', 'bottlethe'}</t>
-  </si>
-  <si>
-    <t>{'greatmy', 'conection', '217was'}</t>
-  </si>
-  <si>
-    <t>{'relaxthere', 'aminta', 'courtsey'}</t>
-  </si>
-  <si>
-    <t>{'aminta', 'itâ€™s', 'day/evening'}</t>
-  </si>
-  <si>
-    <t>{'breakfest', 'aminta'}</t>
-  </si>
-  <si>
-    <t>{'(and', 'iâ€™d', '(this', 'car()', 'late)overall', 'all)', 'itâ€™s'}</t>
-  </si>
-  <si>
-    <t>{'somethingsfood', 'cleanthe', 'veggie', 'shuttle-service'}</t>
+    <t>{'(the', 'journey)'}</t>
+  </si>
+  <si>
+    <t>{'spritz', 'hotelwe', 'aperol', 'usthe', 'lemoncello', 'spritzi', 'dinnertimethe', 'himthey', 'lightsthe'}</t>
+  </si>
+  <si>
+    <t>{'noneall', 'excellentimmaculately', 'alsothe', 'viewbut', 'standardtoiletries', 'aminta'}</t>
+  </si>
+  <si>
+    <t>{'â‚¬20', 'areathe', 'bottlethe'}</t>
+  </si>
+  <si>
+    <t>{'conection', '217was', 'greatmy'}</t>
+  </si>
+  <si>
+    <t>{'aminta', 'courtsey', 'relaxthere'}</t>
+  </si>
+  <si>
+    <t>{'aminta', 'day/evening', 'itâ€™s'}</t>
+  </si>
+  <si>
+    <t>{'aminta', 'breakfest'}</t>
+  </si>
+  <si>
+    <t>{'all)', '(this', 'iâ€™d', 'car()', 'itâ€™s', 'late)overall', '(and'}</t>
+  </si>
+  <si>
+    <t>{'veggie', 'shuttle-service', 'cleanthe', 'somethingsfood'}</t>
   </si>
   <si>
     <t>{'aminta', 'didnt'}</t>
@@ -61,7 +61,7 @@
     <t>{'awesomeawesome'}</t>
   </si>
   <si>
-    <t>{'finallt', 'wifeâ€™s', 'maintenancedo', 'travellerwe', 'caprialthough', 'breathtakingwe', 'worldand', 'coastnaples', 'sorrentoour'}</t>
+    <t>{'sorrentoour', 'worldand', 'finallt', 'wifeâ€™s', 'travellerwe', 'breathtakingwe', 'caprialthough', 'coastnaples', 'maintenancedo'}</t>
   </si>
   <si>
     <t>{'versuvius'}</t>
@@ -70,7 +70,7 @@
     <t>{'walkable', 'do-ablethe'}</t>
   </si>
   <si>
-    <t>{'thereâ€\x9d', 'â€œoh', 'cannot', 'itâ€™s'}</t>
+    <t>{'thereâ€\x9d', 'itâ€™s', 'â€œoh', 'cannot'}</t>
   </si>
   <si>
     <t>{'aminta'}</t>
@@ -79,49 +79,49 @@
     <t>{'bewarethe'}</t>
   </si>
   <si>
-    <t>{'clientele;', 'reasonablethe', 'plateall', 'steepstaff'}</t>
-  </si>
-  <si>
-    <t>{'gardenoh', 'laurenour', 'pathwaysif', 'valuethe', 'vesuviusbreakfast'}</t>
-  </si>
-  <si>
-    <t>{'absoulutely', ':)all', 'kindnessthe'}</t>
+    <t>{'steepstaff', 'clientele;', 'plateall', 'reasonablethe'}</t>
+  </si>
+  <si>
+    <t>{'laurenour', 'gardenoh', 'vesuviusbreakfast', 'valuethe', 'pathwaysif'}</t>
+  </si>
+  <si>
+    <t>{'kindnessthe', ':)all', 'absoulutely'}</t>
   </si>
   <si>
     <t>{'aminta', '60th', 'wifeâ€™s'}</t>
   </si>
   <si>
-    <t>{'themour', 'viewsalthough', 'amintas', 'trainwhen', '(grazie)', 'victorria', 'staffthe', 'perfectionlucai', 'goodbyein', 'standardthe', 'emailed', 'aminta', 'me)', 'hote', 'amintasuzanne', 'enderlin', 'futurethe', 'sorrentoprior', 'michaeli', 'waitwe', 'seawe'}</t>
+    <t>{'enderlin', 'themour', 'staffthe', '(grazie)', 'amintas', 'michaeli', 'goodbyein', 'aminta', 'sorrentoprior', 'emailed', 'waitwe', 'perfectionlucai', 'me)', 'futurethe', 'standardthe', 'seawe', 'trainwhen', 'hote', 'amintasuzanne', 'viewsalthough', 'victorria'}</t>
   </si>
   <si>
     <t>{'wifi'}</t>
   </si>
   <si>
-    <t>{'spectacularwe', 'issues:the', 'wardrobebreakfast'}</t>
+    <t>{'issues:the', 'wardrobebreakfast', 'spectacularwe'}</t>
   </si>
   <si>
     <t>{'amalfii'}</t>
   </si>
   <si>
-    <t>{'(and', 'werent', 'toowe', 'either)', 'didnt'}</t>
-  </si>
-  <si>
-    <t>{'motherâ€™s', 'aminta', 'iâ€™d', 'menu)', 'townthe', 'tripthe', '(mind', 'complexin'}</t>
-  </si>
-  <si>
-    <t>{'aminta', '(and', '14th', 'travelers)', 'pasquales'}</t>
-  </si>
-  <si>
-    <t>{'40th', 'towni', 'curtiousit', 'hoteli', '3:30am'}</t>
+    <t>{'toowe', 'didnt', 'either)', '(and', 'werent'}</t>
+  </si>
+  <si>
+    <t>{'complexin', 'iâ€™d', 'motherâ€™s', 'tripthe', 'townthe', '(mind', 'menu)', 'aminta'}</t>
+  </si>
+  <si>
+    <t>{'travelers)', 'pasquales', 'aminta', '(and', '14th'}</t>
+  </si>
+  <si>
+    <t>{'40th', 'towni', 'hoteli', '3:30am', 'curtiousit'}</t>
   </si>
   <si>
     <t>{'weâ€™ll'}</t>
   </si>
   <si>
-    <t>{'coffeethe', 'couldnâ€™t', '15th'}</t>
-  </si>
-  <si>
-    <t>{'aminta', 'traveled', 'helful', '(off-season)', 'overall--staff', 'in-season', '5-10', '8:30', '9:30'}</t>
+    <t>{'coffeethe', '15th', 'couldnâ€™t'}</t>
+  </si>
+  <si>
+    <t>{'overall--staff', '8:30', '(off-season)', 'in-season', 'aminta', '9:30', 'helful', '5-10', 'traveled'}</t>
   </si>
   <si>
     <t>{'aminta', 'dâ€™'}</t>
@@ -130,25 +130,25 @@
     <t>{'aminta', '"wow"'}</t>
   </si>
   <si>
-    <t>{'weather)', 'weâ€™d', 'yearthe', '12:30-3:00', 'didnâ€™t', 'couldnâ€™t', '(me', '(as', 'daughter)'}</t>
-  </si>
-  <si>
-    <t>{'aminta', 'sunset/sea', 'didnâ€™t', 'hillreally', 'driverwe', 'outside/pool'}</t>
-  </si>
-  <si>
-    <t>{':)', 'couldnâ€™t', 'receptionwe', 'canâ€™t', 'tooi'}</t>
-  </si>
-  <si>
-    <t>{'excellemt', 'viewsndiwn', 'barstaff'}</t>
-  </si>
-  <si>
-    <t>{'course)sorrento', 'dayyou', '(you', 'tripadvisor', 'pastry/bread', 'before)', 'reading)', '(especially', '(where', 'aminta', 'be)', 'down)', 'menu)', 'owner(s)reading', '(this', '(reserved', '(apart', 'nightbreakfast', 'viewsthey'}</t>
-  </si>
-  <si>
-    <t>{'impeccablythe', 'backbreakfast', 'didnâ€™t', 'afterit', 'tippingwe', 'knowledgeablewe', 'hotelthere', 'thinkwe', 'poolall', 'donâ€™t'}</t>
-  </si>
-  <si>
-    <t>{'barstaff/lunch', '4-5', 'â‚¬50', 'folks)', '(remember'}</t>
+    <t>{'yearthe', 'couldnâ€™t', '12:30-3:00', 'didnâ€™t', 'daughter)', 'weather)', '(as', '(me', 'weâ€™d'}</t>
+  </si>
+  <si>
+    <t>{'driverwe', 'didnâ€™t', 'hillreally', 'sunset/sea', 'aminta', 'outside/pool'}</t>
+  </si>
+  <si>
+    <t>{'tooi', ':)', 'couldnâ€™t', 'receptionwe', 'canâ€™t'}</t>
+  </si>
+  <si>
+    <t>{'barstaff', 'viewsndiwn', 'excellemt'}</t>
+  </si>
+  <si>
+    <t>{'before)', 'reading)', '(this', '(you', 'pastry/bread', 'aminta', 'viewsthey', '(especially', 'be)', 'nightbreakfast', 'tripadvisor', '(reserved', 'menu)', '(where', 'down)', 'course)sorrento', 'owner(s)reading', '(apart', 'dayyou'}</t>
+  </si>
+  <si>
+    <t>{'donâ€™t', 'impeccablythe', 'afterit', 'knowledgeablewe', 'didnâ€™t', 'hotelthere', 'tippingwe', 'backbreakfast', 'poolall', 'thinkwe'}</t>
+  </si>
+  <si>
+    <t>{'(remember', 'folks)', 'barstaff/lunch', 'â‚¬50', '4-5'}</t>
   </si>
   <si>
     <t>{'amintathis', 'didnt'}</t>
@@ -163,34 +163,34 @@
     <t>{'100%'}</t>
   </si>
   <si>
-    <t>{'(steeply', 'lantica', 'youre', 'special)we', 'alleys)', 'mornings;', 'pressure;', '5-10', 'tomato)', '(though', 'aminta', '(but', '9:30am', '(although', 'labate', 'meal)', 'favorably', 'bad;', 'didnt', '(we', 'pleasantthe', 'overnight)', 'pastriestheres', 'onein', 'sorento'}</t>
-  </si>
-  <si>
-    <t>{'aminta', 'lotthere', 'thereafterpool'}</t>
+    <t>{'pastriestheres', 'sorento', 'overnight)', 'didnt', '9:30am', 'lantica', '(we', 'labate', 'aminta', '(but', 'alleys)', 'meal)', 'tomato)', 'special)we', 'mornings;', '(although', '(steeply', 'bad;', 'youre', 'onein', 'pleasantthe', 'favorably', '(though', 'pressure;', '5-10'}</t>
+  </si>
+  <si>
+    <t>{'aminta', 'thereafterpool', 'lotthere'}</t>
   </si>
   <si>
     <t>{'aminta', 'couldnâ€™t'}</t>
   </si>
   <si>
-    <t>{'staff;', 'hill:', 'rooms;'}</t>
+    <t>{'hill:', 'rooms;', 'staff;'}</t>
   </si>
   <si>
     <t>{'spaciouse', 'etcas'}</t>
   </si>
   <si>
-    <t>{'wifes', ':)', 'prosecco'}</t>
-  </si>
-  <si>
-    <t>{'wordeverything', 'operatorssuch', '"we', '1970s', 'slimethere', 'tomatoesevery', 'september?', 'why?such', 'plastic"', 'dacampo'}</t>
-  </si>
-  <si>
-    <t>{'sea/mountain/garden', 'couldnâ€™t', 'hotelcom', 'â‚¬174/per'}</t>
+    <t>{'wifes', 'prosecco', ':)'}</t>
+  </si>
+  <si>
+    <t>{'september?', '"we', 'operatorssuch', 'why?such', 'plastic"', '1970s', 'wordeverything', 'dacampo', 'slimethere', 'tomatoesevery'}</t>
+  </si>
+  <si>
+    <t>{'sea/mountain/garden', 'hotelcom', 'â‚¬174/per', 'couldnâ€™t'}</t>
   </si>
   <si>
     <t>{'miscommunication', 'hotel)', '(something'}</t>
   </si>
   <si>
-    <t>{'youâ€™d', 'youâ€™ll', 'thereâ€™s', 'locationsonly', 'itâ€™s', '(for', 'topoverall', 'itrestaurant', 'aminta', 'advisorwarmly', 'iâ€™m', 'startrooms', 'drinkshotel', 'donâ€™t', 'wifi', '(big)', 'clinicalstill', 'honeymoon)', 'canâ€™t'}</t>
+    <t>{'donâ€™t', 'aminta', 'wifi', 'iâ€™m', 'youâ€™d', 'startrooms', 'clinicalstill', 'advisorwarmly', 'locationsonly', 'drinkshotel', '(big)', '(for', 'honeymoon)', 'youâ€™ll', 'topoverall', 'canâ€™t', 'itrestaurant', 'itâ€™s', 'thereâ€™s'}</t>
   </si>
   <si>
     <t>{'5*'}</t>
@@ -199,46 +199,46 @@
     <t>{'freindly', 'areurbishment'}</t>
   </si>
   <si>
-    <t>{'poolwe', 'atmospherethere', 'didnt', 'b&amp;b', 'complainthere'}</t>
-  </si>
-  <si>
-    <t>{'butin', 'nightthe', '900am', 'â£250', 'doorbreakfast', 'that;', 'soundproofing'}</t>
-  </si>
-  <si>
-    <t>{'choices-', 'timei', 'swimthe', 'interestingi', 'dessert/', 'timethere'}</t>
-  </si>
-  <si>
-    <t>{'itâ€™s', 'iâ€™m', '70euros'}</t>
-  </si>
-  <si>
-    <t>{'was/offered', 'werenâ€™t', 'arenâ€™t', 'couldnâ€™t', 'wouldnâ€™t', 'itâ€™s'}</t>
-  </si>
-  <si>
-    <t>{'been)', '(and', 'youre', 'isnt'}</t>
-  </si>
-  <si>
-    <t>{'aminta', '330pm', 'desiredall', 'showerbreakfast', '"sunset', 'anywayvery', 'regiona', '20-25min', 'view"', 'didnt'}</t>
-  </si>
-  <si>
-    <t>{'busthat', 'traveled', 'aminta', 'riveria', 'sorento', 'didnt'}</t>
+    <t>{'complainthere', 'didnt', 'b&amp;b', 'poolwe', 'atmospherethere'}</t>
+  </si>
+  <si>
+    <t>{'900am', 'doorbreakfast', 'nightthe', 'â£250', 'soundproofing', 'butin', 'that;'}</t>
+  </si>
+  <si>
+    <t>{'dessert/', 'timethere', 'interestingi', 'choices-', 'timei', 'swimthe'}</t>
+  </si>
+  <si>
+    <t>{'70euros', 'itâ€™s', 'iâ€™m'}</t>
+  </si>
+  <si>
+    <t>{'was/offered', 'arenâ€™t', 'wouldnâ€™t', 'couldnâ€™t', 'werenâ€™t', 'itâ€™s'}</t>
+  </si>
+  <si>
+    <t>{'youre', '(and', 'been)', 'isnt'}</t>
+  </si>
+  <si>
+    <t>{'showerbreakfast', 'didnt', '"sunset', '330pm', 'anywayvery', 'regiona', 'aminta', 'view"', '20-25min', 'desiredall'}</t>
+  </si>
+  <si>
+    <t>{'sorento', 'didnt', 'riveria', 'aminta', 'traveled', 'busthat'}</t>
   </si>
   <si>
     <t>{'hotelwould'}</t>
   </si>
   <si>
-    <t>{'doesnt', 'unnecesary', 'cabfinal', 'positivesit', 'available?on', 'supplementbest', 'inthis', 'aviod', '9:30', 'eu150', '20-', 'hankerchief', '10:00am', '11:30', 'tiledbreakfasts', 'didnt'}</t>
+    <t>{'doesnt', 'inthis', 'tiledbreakfasts', 'cabfinal', '20-', 'positivesit', '10:00am', '11:30', 'unnecesary', 'didnt', 'eu150', 'supplementbest', 'aviod', '9:30', 'available?on', 'hankerchief'}</t>
   </si>
   <si>
     <t>{'predictableour', 'centrewe', 'jamsone'}</t>
   </si>
   <si>
-    <t>{'hotelâ€™s', 'aminta', 'onthe', 'itâ€™s'}</t>
-  </si>
-  <si>
-    <t>{'milk)', 'betterfood', 'viewsthe', 'bagsroom'}</t>
-  </si>
-  <si>
-    <t>{'10:30', 'points:', 'mediterranean?', 'back?', 'kidsthe', 'areanot', 'worldcharm', 'colleaguegood', 'good:'}</t>
+    <t>{'aminta', 'onthe', 'itâ€™s', 'hotelâ€™s'}</t>
+  </si>
+  <si>
+    <t>{'viewsthe', 'bagsroom', 'milk)', 'betterfood'}</t>
+  </si>
+  <si>
+    <t>{'areanot', 'worldcharm', 'good:', 'kidsthe', 'back?', 'points:', '10:30', 'mediterranean?', 'colleaguegood'}</t>
   </si>
   <si>
     <t>{'brotherthis'}</t>
@@ -247,7 +247,7 @@
     <t>{'7pm', 'had(carbonara'}</t>
   </si>
   <si>
-    <t>{'aminta', 'cannot', 'attentivewe'}</t>
+    <t>{'aminta', 'attentivewe', 'cannot'}</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Case sensitiv Problematik behoben
</commit_message>
<xml_diff>
--- a/Example2.xlsx
+++ b/Example2.xlsx
@@ -14,240 +14,222 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="78">
-  <si>
-    <t>{'dog/dogs'}</t>
-  </si>
-  <si>
-    <t>{'tripscheck', 'vusuviogood'}</t>
-  </si>
-  <si>
-    <t>set()</t>
-  </si>
-  <si>
-    <t>{'(the', 'journey)'}</t>
-  </si>
-  <si>
-    <t>{'dinnertimethe', 'lightsthe', 'spritz', 'spritzi', 'hotelwe', 'himthey', 'lemoncello', 'aperol', 'usthe'}</t>
-  </si>
-  <si>
-    <t>{'standardtoiletries', 'noneall', 'alsothe', 'excellentimmaculately', 'viewbut', 'aminta'}</t>
-  </si>
-  <si>
-    <t>{'bottlethe', 'â‚¬20', 'areathe'}</t>
-  </si>
-  <si>
-    <t>{'conection', 'greatmy', '217was'}</t>
-  </si>
-  <si>
-    <t>{'relaxthere', 'courtsey', 'aminta'}</t>
-  </si>
-  <si>
-    <t>{'itâ€™s', 'day/evening', 'aminta'}</t>
-  </si>
-  <si>
-    <t>{'breakfest', 'aminta'}</t>
-  </si>
-  <si>
-    <t>{'iâ€™d', 'all)', 'itâ€™s', 'late)overall', '(this', 'car()', '(and'}</t>
-  </si>
-  <si>
-    <t>{'shuttle-service', 'cleanthe', 'veggie', 'somethingsfood'}</t>
-  </si>
-  <si>
-    <t>{'aminta', 'didnt'}</t>
-  </si>
-  <si>
-    <t>{'awesomeawesome'}</t>
-  </si>
-  <si>
-    <t>{'maintenancedo', 'worldand', 'breathtakingwe', 'coastnaples', 'wifeâ€™s', 'caprialthough', 'sorrentoour', 'travellerwe', 'finallt'}</t>
-  </si>
-  <si>
-    <t>{'versuvius'}</t>
-  </si>
-  <si>
-    <t>{'do-ablethe', 'walkable'}</t>
-  </si>
-  <si>
-    <t>{'itâ€™s', 'thereâ€\x9d', 'cannot', 'â€œoh'}</t>
-  </si>
-  <si>
-    <t>{'aminta'}</t>
-  </si>
-  <si>
-    <t>{'bewarethe'}</t>
-  </si>
-  <si>
-    <t>{'steepstaff', 'reasonablethe', 'clientele;', 'plateall'}</t>
-  </si>
-  <si>
-    <t>{'valuethe', 'laurenour', 'vesuviusbreakfast', 'gardenoh', 'pathwaysif'}</t>
-  </si>
-  <si>
-    <t>{'absoulutely', ':)all', 'kindnessthe'}</t>
-  </si>
-  <si>
-    <t>{'60th', 'wifeâ€™s', 'aminta'}</t>
-  </si>
-  <si>
-    <t>{'seawe', 'themour', 'me)', 'michaeli', 'emailed', 'trainwhen', 'futurethe', 'staffthe', '(grazie)', 'waitwe', 'sorrentoprior', 'aminta', 'goodbyein', 'victorria', 'standardthe', 'amintasuzanne', 'perfectionlucai', 'viewsalthough', 'hote', 'amintas', 'enderlin'}</t>
-  </si>
-  <si>
-    <t>{'wifi'}</t>
-  </si>
-  <si>
-    <t>{'spectacularwe', 'issues:the', 'wardrobebreakfast'}</t>
-  </si>
-  <si>
-    <t>{'amalfii'}</t>
-  </si>
-  <si>
-    <t>{'either)', 'didnt', 'werent', '(and', 'toowe'}</t>
-  </si>
-  <si>
-    <t>{'iâ€™d', 'tripthe', 'motherâ€™s', 'complexin', 'aminta', 'townthe', 'menu)', '(mind'}</t>
-  </si>
-  <si>
-    <t>{'14th', 'pasquales', 'travelers)', 'aminta', '(and'}</t>
-  </si>
-  <si>
-    <t>{'3:30am', 'curtiousit', '40th', 'towni', 'hoteli'}</t>
-  </si>
-  <si>
-    <t>{'weâ€™ll'}</t>
-  </si>
-  <si>
-    <t>{'couldnâ€™t', 'coffeethe', '15th'}</t>
-  </si>
-  <si>
-    <t>{'9:30', '8:30', 'in-season', 'aminta', 'traveled', 'helful', 'overall--staff', '(off-season)', '5-10'}</t>
-  </si>
-  <si>
-    <t>{'dâ€™', 'aminta'}</t>
-  </si>
-  <si>
-    <t>{'"wow"', 'aminta'}</t>
-  </si>
-  <si>
-    <t>{'12:30-3:00', 'weather)', 'daughter)', 'yearthe', 'weâ€™d', '(as', '(me', 'couldnâ€™t', 'didnâ€™t'}</t>
-  </si>
-  <si>
-    <t>{'hillreally', 'outside/pool', 'sunset/sea', 'aminta', 'driverwe', 'didnâ€™t'}</t>
-  </si>
-  <si>
-    <t>{'canâ€™t', ':)', 'tooi', 'receptionwe', 'couldnâ€™t'}</t>
-  </si>
-  <si>
-    <t>{'excellemt', 'viewsndiwn', 'barstaff'}</t>
-  </si>
-  <si>
-    <t>{'(apart', '(especially', '(where', '(this', 'owner(s)reading', 'dayyou', 'reading)', 'before)', 'down)', 'viewsthey', 'aminta', 'nightbreakfast', 'menu)', '(reserved', 'course)sorrento', 'pastry/bread', 'be)', '(you', 'tripadvisor'}</t>
-  </si>
-  <si>
-    <t>{'backbreakfast', 'thinkwe', 'knowledgeablewe', 'afterit', 'poolall', 'donâ€™t', 'hotelthere', 'tippingwe', 'impeccablythe', 'didnâ€™t'}</t>
-  </si>
-  <si>
-    <t>{'â‚¬50', '(remember', '4-5', 'barstaff/lunch', 'folks)'}</t>
-  </si>
-  <si>
-    <t>{'amintathis', 'didnt'}</t>
-  </si>
-  <si>
-    <t>{'sunset/sea', 'wouldnâ€™t', '50th', 'aminta'}</t>
-  </si>
-  <si>
-    <t>{'(10', 'traffic)', '1960s'}</t>
-  </si>
-  <si>
-    <t>{'100%'}</t>
-  </si>
-  <si>
-    <t>{'tomato)', '(though', '9:30am', 'pleasantthe', '(although', '5-10', 'alleys)', '(but', 'pastriestheres', '(we', 'lantica', 'meal)', 'sorento', 'didnt', 'special)we', 'pressure;', 'favorably', 'aminta', '(steeply', 'youre', 'labate', 'onein', 'overnight)', 'mornings;', 'bad;'}</t>
-  </si>
-  <si>
-    <t>{'thereafterpool', 'aminta', 'lotthere'}</t>
-  </si>
-  <si>
-    <t>{'couldnâ€™t', 'aminta'}</t>
-  </si>
-  <si>
-    <t>{'hill:', 'rooms;', 'staff;'}</t>
-  </si>
-  <si>
-    <t>{'etcas', 'spaciouse'}</t>
-  </si>
-  <si>
-    <t>{'wifes', 'prosecco', ':)'}</t>
-  </si>
-  <si>
-    <t>{'operatorssuch', 'plastic"', 'september?', 'wordeverything', 'slimethere', 'tomatoesevery', 'dacampo', '"we', 'why?such', '1970s'}</t>
-  </si>
-  <si>
-    <t>{'sea/mountain/garden', 'hotelcom', 'couldnâ€™t', 'â‚¬174/per'}</t>
-  </si>
-  <si>
-    <t>{'(something', 'hotel)', 'miscommunication'}</t>
-  </si>
-  <si>
-    <t>{'itâ€™s', 'wifi', 'youâ€™d', '(big)', 'advisorwarmly', 'startrooms', 'itrestaurant', 'locationsonly', 'honeymoon)', 'topoverall', 'iâ€™m', 'youâ€™ll', 'aminta', 'drinkshotel', 'canâ€™t', 'thereâ€™s', '(for', 'donâ€™t', 'clinicalstill'}</t>
-  </si>
-  <si>
-    <t>{'5*'}</t>
-  </si>
-  <si>
-    <t>{'freindly', 'areurbishment'}</t>
-  </si>
-  <si>
-    <t>{'poolwe', 'didnt', 'complainthere', 'b&amp;b', 'atmospherethere'}</t>
-  </si>
-  <si>
-    <t>{'that;', '900am', 'â£250', 'nightthe', 'butin', 'doorbreakfast', 'soundproofing'}</t>
-  </si>
-  <si>
-    <t>{'choices-', 'timethere', 'interestingi', 'swimthe', 'timei', 'dessert/'}</t>
-  </si>
-  <si>
-    <t>{'itâ€™s', 'iâ€™m', '70euros'}</t>
-  </si>
-  <si>
-    <t>{'wouldnâ€™t', 'werenâ€™t', 'itâ€™s', 'arenâ€™t', 'couldnâ€™t', 'was/offered'}</t>
-  </si>
-  <si>
-    <t>{'(and', 'youre', 'isnt', 'been)'}</t>
-  </si>
-  <si>
-    <t>{'view"', 'didnt', '20-25min', 'showerbreakfast', 'aminta', 'desiredall', 'anywayvery', '330pm', '"sunset', 'regiona'}</t>
-  </si>
-  <si>
-    <t>{'sorento', 'didnt', 'riveria', 'aminta', 'traveled', 'busthat'}</t>
-  </si>
-  <si>
-    <t>{'hotelwould'}</t>
-  </si>
-  <si>
-    <t>{'cabfinal', 'doesnt', 'aviod', 'didnt', 'inthis', '9:30', '20-', 'tiledbreakfasts', 'hankerchief', 'positivesit', 'eu150', 'available?on', '11:30', 'unnecesary', '10:00am', 'supplementbest'}</t>
-  </si>
-  <si>
-    <t>{'predictableour', 'centrewe', 'jamsone'}</t>
-  </si>
-  <si>
-    <t>{'itâ€™s', 'hotelâ€™s', 'onthe', 'aminta'}</t>
-  </si>
-  <si>
-    <t>{'betterfood', 'viewsthe', 'milk)', 'bagsroom'}</t>
-  </si>
-  <si>
-    <t>{'good:', 'mediterranean?', '10:30', 'kidsthe', 'back?', 'points:', 'worldcharm', 'areanot', 'colleaguegood'}</t>
-  </si>
-  <si>
-    <t>{'brotherthis'}</t>
-  </si>
-  <si>
-    <t>{'had(carbonara', '7pm'}</t>
-  </si>
-  <si>
-    <t>{'cannot', 'aminta', 'attentivewe'}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>['vusuvio', 'capri', 'gps']</t>
+  </si>
+  <si>
+    <t>['centre', 'Sorrento', 'Sorrento', 'euros']</t>
+  </si>
+  <si>
+    <t>['centre', 'Utd', 'aperol', 'lemoncello']</t>
+  </si>
+  <si>
+    <t>['Aminta', 'Sorrento', 'Aminta']</t>
+  </si>
+  <si>
+    <t>['bottleThe', 'centre', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['wi', 'fi', 'conection', 'wi', 'fi', 'everytime']</t>
+  </si>
+  <si>
+    <t>['Aminta', 'courtsey']</t>
+  </si>
+  <si>
+    <t>['Aminta']</t>
+  </si>
+  <si>
+    <t>['dont', 'Aminta', 'downton', 'ir', 'breakfest', 'ir']</t>
+  </si>
+  <si>
+    <t>['coeliac', 'Sorrento', 'pre']</t>
+  </si>
+  <si>
+    <t>['ok']</t>
+  </si>
+  <si>
+    <t>['centre', 'Sorrento', 'Sorrento', 'centre', 'finallt', 'Amalfi', 'traveller', 'fab']</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'italian', 'european', 'Sorrento', 'im', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'Sorrento', 'Versuvius', "its'"]</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'mins', 'centre', 'sunbed']</t>
+  </si>
+  <si>
+    <t>['GPS']</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'Aminta']</t>
+  </si>
+  <si>
+    <t>['nighter', 'tv']</t>
+  </si>
+  <si>
+    <t>["'international'", 'clientele']</t>
+  </si>
+  <si>
+    <t>['focussed', "neighbour's"]</t>
+  </si>
+  <si>
+    <t>['absoulutely']</t>
+  </si>
+  <si>
+    <t>['Aminta', 'sorrento', 'Sorrento', 'Aminta']</t>
+  </si>
+  <si>
+    <t>['Aminta', 'Aminta', 'Sorrento', 'Lucai', 'Victorria', 'Michaeli', "Aminta's", 'centre', 'Sorrento', 'Sorrento', 'hote', 'Nino', "'hello'", 'Aminta', 'Grazie', 'Sorrento', 'Aminta', 'Enderlin']</t>
+  </si>
+  <si>
+    <t>['WiFi', 'centre', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['wardrobebreakfast']</t>
+  </si>
+  <si>
+    <t>['Amalfii']</t>
+  </si>
+  <si>
+    <t>['neighbouring', 'Sorrento', 'centre', 'Sorrento', 'Sorrento', 'centre', 'Sorrento', 'Sorrento', 'sunbed', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['Aminta', 'travellers', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['organise', 'curtious', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'centre', 'couldn']</t>
+  </si>
+  <si>
+    <t>['Aminta', 'helful', 'Sorrento', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['Aminta', 'maitre']</t>
+  </si>
+  <si>
+    <t>['sorrento', 'aminta']</t>
+  </si>
+  <si>
+    <t>['samey', 'couldn', 'didn', 'didn', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['Aminta', 'didn', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['couldn']</t>
+  </si>
+  <si>
+    <t>['barstaff', 'excellemt', 'viewsndiwn', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'centre', 'sunbeds', 'Euros', 'Aminta', 'TripAdvisor', 'Sorrento', 'Amalfi', 'Positano', 'Ravello', 'Harbour']</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'didn', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['sunbeds', 'Sorrento', 'barstaff', "'stuck'", 'mins']</t>
+  </si>
+  <si>
+    <t>['Aminta', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'wouldn', 'Aminta', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'mins', "'s"]</t>
+  </si>
+  <si>
+    <t>['Sorrento']</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'wifi']</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'Sorrento', 'Sorento', 'Sorento', "l'Abate", 'Porta', 'Grande', "l'Antica", 'Trattoria', 'Aminta', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'centre', 'Sorrento', 'Aminta', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['Couldn', 'Aminta']</t>
+  </si>
+  <si>
+    <t>['sunbeds']</t>
+  </si>
+  <si>
+    <t>['spaciouse']</t>
+  </si>
+  <si>
+    <t>['maitre', 'prosecco']</t>
+  </si>
+  <si>
+    <t>['unrecognisable', 'flavours', 'Maitre', "d'", "'s", 'Merlot', 'Sorrento', "d'Acampo"]</t>
+  </si>
+  <si>
+    <t>['Positano', 'accomodation', 'Aminta', 'Sorrento', 'wifi']</t>
+  </si>
+  <si>
+    <t>['centre', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['freindly', 'areurbishment']</t>
+  </si>
+  <si>
+    <t>['tv']</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'swimThe']</t>
+  </si>
+  <si>
+    <t>['Euros', 'wil', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['weren', 'Euros', 'aren', 'couldn', 'Wouldn']</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'Sorrento']</t>
+  </si>
+  <si>
+    <t>['Sorrento', 'Amalfi', 'Aminta']</t>
+  </si>
+  <si>
+    <t>['til']</t>
+  </si>
+  <si>
+    <t>['Riveria', 'Aminta', 'busThat', 'Sorento', 'mins']</t>
+  </si>
+  <si>
+    <t>['Amalfi', 'clientele']</t>
+  </si>
+  <si>
+    <t>['LOved']</t>
+  </si>
+  <si>
+    <t>['hankerchief', "'safe'", 'mellon', 'Euros', 'unnecesary', 'Euro', 'aviod']</t>
+  </si>
+  <si>
+    <t>['sunbed', 'sunbeds', 'Sorrento', 'Sorrento', 'Aminta']</t>
+  </si>
+  <si>
+    <t>['judgement', 'Sorrento', 'centre']</t>
+  </si>
+  <si>
+    <t>['Euros']</t>
+  </si>
+  <si>
+    <t>['euros', "Tesco's", 'Sorrento', 'worldCharm']</t>
+  </si>
+  <si>
+    <t>['bc', 'ok', 'carbonara']</t>
   </si>
 </sst>
 </file>
@@ -590,10 +572,10 @@
         <v>0</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="2:4">
@@ -601,15 +583,15 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -620,62 +602,62 @@
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>9</v>
-      </c>
       <c r="D5">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -686,7 +668,7 @@
     </row>
     <row r="10" spans="2:4">
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -697,21 +679,21 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D11">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>82</v>
@@ -719,7 +701,7 @@
     </row>
     <row r="13" spans="2:4">
       <c r="B13" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -730,21 +712,21 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>42</v>
@@ -752,10 +734,10 @@
     </row>
     <row r="16" spans="2:4">
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D16">
         <v>301</v>
@@ -763,10 +745,10 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>154</v>
@@ -774,10 +756,10 @@
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>144</v>
@@ -785,76 +767,76 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D21">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D22">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25">
         <v>53</v>
@@ -862,21 +844,21 @@
     </row>
     <row r="26" spans="2:4">
       <c r="B26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D27">
         <v>133</v>
@@ -884,18 +866,18 @@
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C28">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -906,62 +888,62 @@
     </row>
     <row r="30" spans="2:4">
       <c r="B30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D31">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="B32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C32">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D32">
-        <v>396</v>
+        <v>407</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D33">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="B34" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D34">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -972,32 +954,32 @@
     </row>
     <row r="36" spans="2:4">
       <c r="B36" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D36">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C37">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D37">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D38">
         <v>63</v>
@@ -1005,21 +987,21 @@
     </row>
     <row r="39" spans="2:4">
       <c r="B39" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D39">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40">
         <v>82</v>
@@ -1027,18 +1009,18 @@
     </row>
     <row r="41" spans="2:4">
       <c r="B41" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1049,29 +1031,29 @@
     </row>
     <row r="43" spans="2:4">
       <c r="B43" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C43">
         <v>3</v>
       </c>
       <c r="D43">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="2:4">
       <c r="B44" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C44">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D44">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="2:4">
       <c r="B45" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -1082,51 +1064,51 @@
     </row>
     <row r="46" spans="2:4">
       <c r="B46" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C46">
         <v>2</v>
       </c>
       <c r="D46">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C47">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D47">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="B48" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C48">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D48">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="49" spans="2:4">
       <c r="B49" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C49">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D49">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="2:4">
       <c r="B50" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1137,10 +1119,10 @@
     </row>
     <row r="51" spans="2:4">
       <c r="B51" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C51">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D51">
         <v>34</v>
@@ -1148,7 +1130,7 @@
     </row>
     <row r="52" spans="2:4">
       <c r="B52" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -1159,51 +1141,51 @@
     </row>
     <row r="53" spans="2:4">
       <c r="B53" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C53">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D53">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="54" spans="2:4">
       <c r="B54" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C54">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D54">
-        <v>272</v>
+        <v>282</v>
       </c>
     </row>
     <row r="55" spans="2:4">
       <c r="B55" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C55">
         <v>5</v>
       </c>
       <c r="D55">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="56" spans="2:4">
       <c r="B56" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C56">
         <v>2</v>
       </c>
       <c r="D56">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="2:4">
       <c r="B57" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C57">
         <v>4</v>
@@ -1214,98 +1196,98 @@
     </row>
     <row r="58" spans="2:4">
       <c r="B58" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C58">
         <v>3</v>
       </c>
       <c r="D58">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="B59" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="2:4">
       <c r="B60" t="s">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="2:4">
       <c r="B61" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D61">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="2:4">
       <c r="B62" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C62">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D62">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="63" spans="2:4">
       <c r="B63" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D63">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C64">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D64">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="2:4">
       <c r="B65" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C65">
         <v>2</v>
       </c>
       <c r="D65">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="2:4">
       <c r="B66" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="C66">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D66">
         <v>72</v>
@@ -1313,142 +1295,142 @@
     </row>
     <row r="67" spans="2:4">
       <c r="B67" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="2:4">
       <c r="B68" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D68">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="2:4">
       <c r="B69" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D69">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="2:4">
       <c r="B70" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="71" spans="2:4">
       <c r="B71" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C71">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D71">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="72" spans="2:4">
       <c r="B72" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C72">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D72">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="2:4">
       <c r="B73" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C73">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D73">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="74" spans="2:4">
       <c r="B74" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C74">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D74">
-        <v>296</v>
+        <v>312</v>
       </c>
     </row>
     <row r="75" spans="2:4">
       <c r="B75" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D75">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="2:4">
       <c r="B76" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C76">
         <v>2</v>
       </c>
       <c r="D76">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="77" spans="2:4">
       <c r="B77" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C77">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D77">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="78" spans="2:4">
       <c r="B78" t="s">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="C78">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D78">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="79" spans="2:4">
       <c r="B79" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79">
         <v>99</v>
@@ -1456,10 +1438,10 @@
     </row>
     <row r="80" spans="2:4">
       <c r="B80" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80">
         <v>37</v>
@@ -1467,43 +1449,43 @@
     </row>
     <row r="81" spans="2:4">
       <c r="B81" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C81">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D81">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="82" spans="2:4">
       <c r="B82" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C82">
         <v>3</v>
       </c>
       <c r="D82">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="83" spans="2:4">
       <c r="B83" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C83">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D83">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="84" spans="2:4">
       <c r="B84" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C84">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D84">
         <v>81</v>
@@ -1511,21 +1493,21 @@
     </row>
     <row r="85" spans="2:4">
       <c r="B85" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C85">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D85">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="86" spans="2:4">
       <c r="B86" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86">
         <v>33</v>
@@ -1533,29 +1515,29 @@
     </row>
     <row r="87" spans="2:4">
       <c r="B87" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C87">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D87">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="88" spans="2:4">
       <c r="B88" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D88">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="89" spans="2:4">
       <c r="B89" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -1566,32 +1548,32 @@
     </row>
     <row r="90" spans="2:4">
       <c r="B90" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C90">
         <v>1</v>
       </c>
       <c r="D90">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="91" spans="2:4">
       <c r="B91" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C91">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D91">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="92" spans="2:4">
       <c r="B92" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="C92">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D92">
         <v>363</v>
@@ -1599,40 +1581,40 @@
     </row>
     <row r="93" spans="2:4">
       <c r="B93" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C93">
         <v>3</v>
       </c>
       <c r="D93">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="94" spans="2:4">
       <c r="B94" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="C94">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D94">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="95" spans="2:4">
       <c r="B95" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C95">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D95">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="96" spans="2:4">
       <c r="B96" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -1643,32 +1625,32 @@
     </row>
     <row r="97" spans="2:4">
       <c r="B97" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C97">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D97">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="98" spans="2:4">
       <c r="B98" t="s">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D98">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="99" spans="2:4">
       <c r="B99" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C99">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D99">
         <v>96</v>
@@ -1676,13 +1658,13 @@
     </row>
     <row r="100" spans="2:4">
       <c r="B100" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="C100">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D100">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>